<commit_message>
add and update data
</commit_message>
<xml_diff>
--- a/QUBE/examples/Inverted_Pendulum_data/data3.xlsx
+++ b/QUBE/examples/Inverted_Pendulum_data/data3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NTNU\AIS4002\Pendulum_RL\QUBE\examples\Inverted_Pendulum_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NTNU\Pendulum_RL\QUBE\examples\Inverted_Pendulum_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11FDBB6E-831E-47FC-81C5-7F7D8E87E17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FB180B-01DB-4FEB-AD0F-9244871A4EA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41055" yWindow="-21855" windowWidth="12165" windowHeight="14805" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23280" yWindow="9195" windowWidth="18135" windowHeight="21975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="2023">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2024" uniqueCount="2024">
+  <si>
+    <t>time,position,angle,motor_velocity,pendulum_velocity,voltage,energy,mode</t>
+  </si>
   <si>
     <t>2995,-12.00,127.27,0.00,351.56,-0.42,0.05,0</t>
   </si>
@@ -6411,10 +6414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A2023"/>
+  <dimension ref="A1:A2024"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16534,6 +16537,11 @@
         <v>2022</v>
       </c>
     </row>
+    <row r="2024" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2024" t="s">
+        <v>2023</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>